<commit_message>
valuation of kalika mandir & bindabaasini mandir
</commit_message>
<xml_diff>
--- a/ofc/estimates/badri dai ko wall/badri dai ko wall.xlsx
+++ b/ofc/estimates/badri dai ko wall/badri dai ko wall.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\badri dai ko wall\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\badri dai ko wall\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -36,15 +36,15 @@
     <definedName name="description_312">[4]Abstract!$B$61</definedName>
     <definedName name="description_5">[1]Abstract!$B$171</definedName>
     <definedName name="description_6">[3]Abstract!$B$172</definedName>
-    <definedName name="description_706">[6]Abstract!$B$265</definedName>
+    <definedName name="description_706">[5]Abstract!$B$265</definedName>
     <definedName name="description_759">[1]Abstract!$B$278</definedName>
-    <definedName name="description_781">[5]Abstract!$B$299</definedName>
+    <definedName name="description_781">[6]Abstract!$B$299</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">estimate!$A$1:$K$62</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">estimate!$A$1:$K$63</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">estimate!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -269,16 +269,19 @@
   </si>
   <si>
     <t>Laying and fixing of Geo-Textile all complete as per specification., Providing  and laying of a geotextile filter between pitching and embankment slopes as per Drawing and Technical Specifications.</t>
+  </si>
+  <si>
+    <t>-for geotextile laying</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -441,7 +444,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -451,7 +454,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,14 +474,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -487,7 +490,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -512,7 +515,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,7 +548,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -554,7 +557,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -569,7 +572,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -585,11 +588,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,8 +601,26 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -625,22 +646,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -652,21 +670,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -989,33 +992,33 @@
       <sheetName val="PPMO_BOQ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="299">
-          <cell r="B299" t="str">
-            <v>Random Rubble Masonry, Providing and laying of Stone Masonry Work in Cement Mortar 1:4 in Foundation complete as per Drawing and Technical Specifications.</v>
+        <row r="265">
+          <cell r="B265" t="str">
+            <v>Laying and fixing of Geo-Textile all complete as per specification., Providing  and laying of a geotextile filter between pitching and embankment slopes as per Drawing and Technical Specifications.</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1050,9 +1053,9 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
-        <row r="265">
-          <cell r="B265" t="str">
-            <v>Laying and fixing of Geo-Textile all complete as per specification., Providing  and laying of a geotextile filter between pitching and embankment slopes as per Drawing and Technical Specifications.</v>
+        <row r="299">
+          <cell r="B299" t="str">
+            <v>Random Rubble Masonry, Providing and laying of Stone Masonry Work in Cement Mortar 1:4 in Foundation complete as per Drawing and Technical Specifications.</v>
           </cell>
         </row>
       </sheetData>
@@ -1349,106 +1352,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="80" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="81" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="82" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="77" t="e">
+      <c r="C6" s="69" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1456,90 +1459,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="77" t="e">
+      <c r="J6" s="69" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="78"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="70"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="I7" s="73" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="71" t="e">
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="77" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="I8" s="74" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="I8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="75" t="e">
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="I9" s="74" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="69" t="s">
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="69" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="K11" s="76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="69"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1558,10 +1561,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="75"/>
+      <c r="K12" s="76"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1604,7 +1607,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="33" t="e">
         <f>#REF!</f>
@@ -1626,7 +1629,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -1639,7 +1642,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1682,7 +1685,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -1695,7 +1698,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1721,13 +1724,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1741,6 +1737,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1756,139 +1759,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U119"/>
+  <dimension ref="A1:U120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="90" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+    </row>
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="81" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-    </row>
-    <row r="5" spans="1:21" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="88" t="s">
+      <c r="H6" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
       <c r="O6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+    </row>
+    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1926,7 +1929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="138" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="38" t="s">
         <v>62</v>
@@ -1958,17 +1961,17 @@
         <v>1</v>
       </c>
       <c r="D10" s="39">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="E10" s="39">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10" s="39">
         <v>0.15</v>
       </c>
       <c r="G10" s="40">
         <f>PRODUCT(C10:F10)</f>
-        <v>5.3999999999999995</v>
+        <v>4.875</v>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="41"/>
@@ -1982,29 +1985,30 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="23">
-        <f>SUM(G10:G10)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="23">
-        <v>64.63</v>
-      </c>
-      <c r="J11" s="42">
-        <f>G11*I11</f>
-        <v>349.00199999999995</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C11" s="37">
+        <v>1</v>
+      </c>
+      <c r="D11" s="39">
+        <v>3</v>
+      </c>
+      <c r="E11" s="39">
+        <v>1</v>
+      </c>
+      <c r="F11" s="39">
+        <v>1</v>
+      </c>
+      <c r="G11" s="40">
+        <f>PRODUCT(C11:F11)</f>
+        <v>3</v>
+      </c>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
       <c r="K11" s="21"/>
       <c r="M11" s="25"/>
       <c r="N11" s="1"/>
@@ -2014,21 +2018,28 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
+      <c r="G12" s="23">
+        <f>SUM(G10:G11)</f>
+        <v>7.875</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="23">
+        <v>64.63</v>
+      </c>
       <c r="J12" s="42">
-        <f>0.13*G11*19284/360</f>
-        <v>37.603799999999993</v>
+        <f>G12*I12</f>
+        <v>508.96124999999995</v>
       </c>
       <c r="K12" s="21"/>
       <c r="M12" s="25"/>
@@ -2039,9 +2050,11 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="38"/>
+      <c r="B13" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
@@ -2049,7 +2062,10 @@
       <c r="G13" s="23"/>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
-      <c r="J13" s="42"/>
+      <c r="J13" s="42">
+        <f>0.13*G12*19284/360</f>
+        <v>54.838874999999994</v>
+      </c>
       <c r="K13" s="21"/>
       <c r="M13" s="25"/>
       <c r="N13" s="1"/>
@@ -2059,13 +2075,9 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:21" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
-        <v>5</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>44</v>
-      </c>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
@@ -2077,98 +2089,106 @@
       <c r="K14" s="21"/>
       <c r="M14" s="25"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="87" t="s">
-        <v>57</v>
-      </c>
-      <c r="P14" s="87"/>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="87"/>
-      <c r="S14" s="87"/>
-      <c r="T14" s="87"/>
-      <c r="U14" s="87"/>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="38" t="str">
-        <f>B20</f>
-        <v>-For stone masonary</v>
-      </c>
-      <c r="C15" s="48">
-        <v>1</v>
-      </c>
-      <c r="D15" s="39">
-        <f>D10</f>
-        <v>6</v>
-      </c>
-      <c r="E15" s="39">
-        <f>E10</f>
-        <v>6</v>
-      </c>
-      <c r="F15" s="39">
-        <v>0.15</v>
-      </c>
-      <c r="G15" s="40">
-        <f>PRODUCT(C15:F15)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+    </row>
+    <row r="15" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>2</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="42"/>
       <c r="K15" s="21"/>
       <c r="M15" s="25"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
-      <c r="B16" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="34">
-        <f>SUM(G15)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="34">
-        <v>4434.5200000000004</v>
-      </c>
-      <c r="J16" s="45">
-        <f>G16*I16</f>
-        <v>23946.407999999999</v>
-      </c>
-      <c r="K16" s="37"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O15" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
+      <c r="R15" s="83"/>
+      <c r="S15" s="83"/>
+      <c r="T15" s="83"/>
+      <c r="U15" s="83"/>
+    </row>
+    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="38" t="str">
+        <f>B21</f>
+        <v>-For stone masonary</v>
+      </c>
+      <c r="C16" s="48">
+        <v>1</v>
+      </c>
+      <c r="D16" s="39">
+        <f>D10</f>
+        <v>6.5</v>
+      </c>
+      <c r="E16" s="39">
+        <f>E10</f>
+        <v>5</v>
+      </c>
+      <c r="F16" s="39">
+        <v>0.15</v>
+      </c>
+      <c r="G16" s="40">
+        <f>PRODUCT(C16:F16)</f>
+        <v>4.875</v>
+      </c>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="21"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C17" s="43"/>
       <c r="D17" s="44"/>
       <c r="E17" s="44"/>
       <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="46">
-        <f>0.13*G16*(14817.6/5)</f>
-        <v>2080.39104</v>
+      <c r="G17" s="34">
+        <f>SUM(G16)</f>
+        <v>4.875</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="34">
+        <v>4434.5200000000004</v>
+      </c>
+      <c r="J17" s="45">
+        <f>G17*I17</f>
+        <v>21618.285000000003</v>
       </c>
       <c r="K17" s="37"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
-      <c r="B18" s="38"/>
+      <c r="B18" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" s="43"/>
       <c r="D18" s="44"/>
       <c r="E18" s="44"/>
@@ -2176,58 +2196,40 @@
       <c r="G18" s="44"/>
       <c r="H18" s="44"/>
       <c r="I18" s="44"/>
-      <c r="J18" s="46"/>
+      <c r="J18" s="46">
+        <f>0.13*G17*(14817.6/5)</f>
+        <v>1878.1308000000001</v>
+      </c>
       <c r="K18" s="37"/>
     </row>
-    <row r="19" spans="1:19" ht="69" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
-        <v>6</v>
-      </c>
-      <c r="B19" s="30" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="41"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="37"/>
+    </row>
+    <row r="20" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>3</v>
+      </c>
+      <c r="B20" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="21"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-    </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="48">
-        <v>1</v>
-      </c>
-      <c r="D20" s="39">
-        <f>D26</f>
-        <v>15</v>
-      </c>
-      <c r="E20" s="39">
-        <v>0.45</v>
-      </c>
-      <c r="F20" s="39">
-        <v>0.05</v>
-      </c>
-      <c r="G20" s="40">
-        <f>PRODUCT(C20:F20)</f>
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="42"/>
       <c r="K20" s="21"/>
       <c r="M20" s="25"/>
       <c r="N20" s="1"/>
@@ -2237,15 +2239,17 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
-      <c r="B21" s="38"/>
+      <c r="B21" s="38" t="s">
+        <v>56</v>
+      </c>
       <c r="C21" s="48">
         <v>1</v>
       </c>
       <c r="D21" s="39">
         <f>D27</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E21" s="39">
         <v>0.45</v>
@@ -2255,7 +2259,7 @@
       </c>
       <c r="G21" s="40">
         <f>PRODUCT(C21:F21)</f>
-        <v>0.1575</v>
+        <v>0.33750000000000002</v>
       </c>
       <c r="H21" s="41"/>
       <c r="I21" s="41"/>
@@ -2269,52 +2273,68 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41"/>
-      <c r="B22" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="34">
-        <f>SUM(G20:G21)</f>
-        <v>0.495</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="34">
-        <v>10634.5</v>
-      </c>
-      <c r="J22" s="45">
-        <f>G22*I22</f>
-        <v>5264.0775000000003</v>
-      </c>
-      <c r="K22" s="37"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="48">
+        <v>1</v>
+      </c>
+      <c r="D22" s="39">
+        <f>D28</f>
+        <v>7</v>
+      </c>
+      <c r="E22" s="39">
+        <v>0.45</v>
+      </c>
+      <c r="F22" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="G22" s="40">
+        <f>PRODUCT(C22:F22)</f>
+        <v>0.1575</v>
+      </c>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="21"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+    </row>
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C23" s="43"/>
       <c r="D23" s="44"/>
       <c r="E23" s="44"/>
       <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="46">
-        <f>0.13*G22*((114907.3+6135.3)/15)</f>
-        <v>519.27275400000008</v>
+      <c r="G23" s="34">
+        <f>SUM(G21:G22)</f>
+        <v>0.495</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="34">
+        <v>10634.5</v>
+      </c>
+      <c r="J23" s="45">
+        <f>G23*I23</f>
+        <v>5264.0775000000003</v>
       </c>
       <c r="K23" s="37"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41"/>
-      <c r="B24" s="38"/>
+      <c r="B24" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C24" s="43"/>
       <c r="D24" s="44"/>
       <c r="E24" s="44"/>
@@ -2322,67 +2342,52 @@
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
       <c r="I24" s="44"/>
-      <c r="J24" s="46"/>
+      <c r="J24" s="46">
+        <f>0.13*G23*((114907.3+6135.3)/15)</f>
+        <v>519.27275400000008</v>
+      </c>
       <c r="K24" s="37"/>
     </row>
-    <row r="25" spans="1:19" s="1" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="64">
-        <v>7</v>
-      </c>
-      <c r="B25" s="30" t="s">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="41"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="37"/>
+    </row>
+    <row r="26" spans="1:19" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="64">
+        <v>4</v>
+      </c>
+      <c r="B26" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="29"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="38" t="s">
+      <c r="C26" s="65"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="29"/>
+    </row>
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="48">
-        <v>1</v>
-      </c>
-      <c r="D26" s="39">
-        <v>15</v>
-      </c>
-      <c r="E26" s="39">
-        <v>0.45</v>
-      </c>
-      <c r="F26" s="39">
-        <v>0.75</v>
-      </c>
-      <c r="G26" s="40">
-        <f>PRODUCT(C26:F26)</f>
-        <v>5.0625</v>
-      </c>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="21"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="38"/>
       <c r="C27" s="48">
         <v>1</v>
       </c>
       <c r="D27" s="39">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E27" s="39">
         <v>0.45</v>
@@ -2392,7 +2397,7 @@
       </c>
       <c r="G27" s="40">
         <f>PRODUCT(C27:F27)</f>
-        <v>2.3624999999999998</v>
+        <v>5.0625</v>
       </c>
       <c r="H27" s="41"/>
       <c r="I27" s="41"/>
@@ -2406,129 +2411,132 @@
       <c r="R27" s="25"/>
       <c r="S27" s="25"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="41"/>
-      <c r="B28" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="34">
-        <f>SUM(G26:G27)</f>
-        <v>7.4249999999999998</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I28" s="34">
-        <v>9709.43</v>
-      </c>
-      <c r="J28" s="45">
-        <f>G28*I28</f>
-        <v>72092.517749999999</v>
-      </c>
-      <c r="K28" s="37"/>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="48">
+        <v>1</v>
+      </c>
+      <c r="D28" s="39">
+        <v>7</v>
+      </c>
+      <c r="E28" s="39">
+        <v>0.45</v>
+      </c>
+      <c r="F28" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="G28" s="40">
+        <f>PRODUCT(C28:F28)</f>
+        <v>2.3624999999999998</v>
+      </c>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="21"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="41"/>
       <c r="B29" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="44"/>
       <c r="E29" s="44"/>
       <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="46">
-        <f>0.13*G28*((27092.1)/5)</f>
-        <v>5230.1299050000007</v>
+      <c r="G29" s="34">
+        <f>SUM(G27:G28)</f>
+        <v>7.4249999999999998</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="34">
+        <v>9709.43</v>
+      </c>
+      <c r="J29" s="45">
+        <f>G29*I29</f>
+        <v>72092.517749999999</v>
       </c>
       <c r="K29" s="37"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41"/>
-      <c r="B30" s="38"/>
+      <c r="B30" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C30" s="43"/>
       <c r="D30" s="44"/>
       <c r="E30" s="44"/>
       <c r="F30" s="44"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="45"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="46">
+        <f>0.13*G29*((27092.1)/5)</f>
+        <v>5230.1299050000007</v>
+      </c>
       <c r="K30" s="37"/>
     </row>
-    <row r="31" spans="1:19" ht="69" x14ac:dyDescent="0.3">
-      <c r="A31" s="18">
-        <v>10</v>
-      </c>
-      <c r="B31" s="30" t="s">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="37"/>
+    </row>
+    <row r="32" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
+        <v>5</v>
+      </c>
+      <c r="B32" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="66" t="s">
+      <c r="D32" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="67" t="s">
+      <c r="E32" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="67" t="s">
+      <c r="F32" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="67" t="s">
+      <c r="G32" s="67" t="s">
         <v>60</v>
-      </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="21"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="19">
-        <f>TRUNC(D33/0.15,0)</f>
-        <v>39</v>
-      </c>
-      <c r="D32" s="20">
-        <f>D10-0.1</f>
-        <v>5.9</v>
-      </c>
-      <c r="E32" s="21">
-        <f>10*10/162</f>
-        <v>0.61728395061728392</v>
-      </c>
-      <c r="F32" s="21">
-        <f>PRODUCT(C32:E32)</f>
-        <v>142.03703703703704</v>
-      </c>
-      <c r="G32" s="68">
-        <f>F32/1000</f>
-        <v>0.14203703703703704</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="23"/>
       <c r="J32" s="42"/>
       <c r="K32" s="21"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
-      <c r="B33" s="38"/>
+      <c r="B33" s="38" t="s">
+        <v>63</v>
+      </c>
       <c r="C33" s="19">
-        <f>TRUNC(D32/0.15,0)</f>
-        <v>39</v>
+        <f>TRUNC(D34/0.15,0)</f>
+        <v>32</v>
       </c>
       <c r="D33" s="20">
-        <f>E10-0.1</f>
-        <v>5.9</v>
+        <f>D10-0.1</f>
+        <v>6.4</v>
       </c>
       <c r="E33" s="21">
         <f>10*10/162</f>
@@ -2536,63 +2544,75 @@
       </c>
       <c r="F33" s="21">
         <f>PRODUCT(C33:E33)</f>
-        <v>142.03703703703704</v>
+        <v>126.41975308641975</v>
       </c>
       <c r="G33" s="68">
         <f>F33/1000</f>
-        <v>0.14203703703703704</v>
+        <v>0.12641975308641976</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="23"/>
       <c r="J33" s="42"/>
       <c r="K33" s="21"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="19">
+        <f>TRUNC(D33/0.15,0)</f>
         <v>42</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="23">
-        <f>SUM(G32:G33)</f>
-        <v>0.28407407407407409</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I34" s="23">
-        <v>124140</v>
-      </c>
-      <c r="J34" s="42">
-        <f>G34*I34</f>
-        <v>35264.955555555556</v>
-      </c>
+      <c r="D34" s="20">
+        <f>E10-0.1</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E34" s="21">
+        <f>10*10/162</f>
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="F34" s="21">
+        <f>PRODUCT(C34:E34)</f>
+        <v>127.03703703703704</v>
+      </c>
+      <c r="G34" s="68">
+        <f>F34/1000</f>
+        <v>0.12703703703703703</v>
+      </c>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="42"/>
       <c r="K34" s="21"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="20"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="23"/>
+      <c r="G35" s="23">
+        <f>SUM(G33:G34)</f>
+        <v>0.25345679012345679</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I35" s="23">
+        <v>124140</v>
+      </c>
       <c r="J35" s="42">
-        <f>0.13*G34*110960</f>
-        <v>4097.7117037037042</v>
+        <f>G35*I35</f>
+        <v>31464.125925925924</v>
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
-      <c r="B36" s="38"/>
+      <c r="B36" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C36" s="19"/>
       <c r="D36" s="20"/>
       <c r="E36" s="21"/>
@@ -2600,14 +2620,15 @@
       <c r="G36" s="23"/>
       <c r="H36" s="22"/>
       <c r="I36" s="23"/>
-      <c r="J36" s="42"/>
+      <c r="J36" s="42">
+        <f>0.13*G35*110960</f>
+        <v>3656.0635061728399</v>
+      </c>
       <c r="K36" s="21"/>
     </row>
-    <row r="37" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
-      <c r="B37" s="30" t="s">
-        <v>66</v>
-      </c>
+      <c r="B37" s="38"/>
       <c r="C37" s="19"/>
       <c r="D37" s="20"/>
       <c r="E37" s="21"/>
@@ -2618,187 +2639,188 @@
       <c r="J37" s="42"/>
       <c r="K37" s="21"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="38" t="str">
+    <row r="38" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>6</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="21"/>
+    </row>
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="38" t="str">
         <f>B10</f>
         <v>-for road</v>
       </c>
-      <c r="C38" s="48">
+      <c r="C39" s="48">
         <v>1</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D39" s="39">
         <f>D10</f>
-        <v>6</v>
-      </c>
-      <c r="E38" s="39">
+        <v>6.5</v>
+      </c>
+      <c r="E39" s="39">
         <f>E10</f>
-        <v>6</v>
-      </c>
-      <c r="F38" s="39">
+        <v>5</v>
+      </c>
+      <c r="F39" s="39">
         <v>0.15</v>
       </c>
-      <c r="G38" s="40">
-        <f>PRODUCT(C38:F38)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="21"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="25"/>
-      <c r="S38" s="25"/>
-    </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="41"/>
-      <c r="B39" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="34">
-        <f>SUM(G38:G38)</f>
-        <v>5.3999999999999995</v>
-      </c>
-      <c r="H39" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I39" s="34">
-        <v>11588.17</v>
-      </c>
-      <c r="J39" s="45">
-        <f>G39*I39</f>
-        <v>62576.117999999995</v>
-      </c>
-      <c r="K39" s="37"/>
-    </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="40">
+        <f>PRODUCT(C39:F39)</f>
+        <v>4.875</v>
+      </c>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="21"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41"/>
       <c r="B40" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C40" s="43"/>
       <c r="D40" s="44"/>
       <c r="E40" s="44"/>
       <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="46">
-        <f>0.13*G39*(128662.2+6685.5)/15</f>
-        <v>6334.2723599999999</v>
+      <c r="G40" s="34">
+        <f>SUM(G39:G39)</f>
+        <v>4.875</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I40" s="34">
+        <v>11588.17</v>
+      </c>
+      <c r="J40" s="45">
+        <f>G40*I40</f>
+        <v>56492.328750000001</v>
       </c>
       <c r="K40" s="37"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41"/>
-      <c r="B41" s="38"/>
+      <c r="B41" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C41" s="43"/>
       <c r="D41" s="44"/>
       <c r="E41" s="44"/>
       <c r="F41" s="44"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="45"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="46">
+        <f>0.13*G40*(128662.2+6685.5)/15</f>
+        <v>5718.4403250000014</v>
+      </c>
       <c r="K41" s="37"/>
     </row>
-    <row r="42" spans="1:19" ht="193.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="18">
-        <v>11</v>
-      </c>
-      <c r="B42" s="30" t="s">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="41"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="37"/>
+    </row>
+    <row r="43" spans="1:19" ht="225" x14ac:dyDescent="0.25">
+      <c r="A43" s="18">
+        <v>7</v>
+      </c>
+      <c r="B43" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="21"/>
-    </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="19">
-        <v>1</v>
-      </c>
-      <c r="D43" s="39">
-        <v>3</v>
-      </c>
-      <c r="E43" s="39">
-        <v>1</v>
-      </c>
-      <c r="F43" s="39">
-        <v>1</v>
-      </c>
-      <c r="G43" s="40">
-        <f t="shared" ref="G43" si="0">PRODUCT(C43:F43)</f>
-        <v>3</v>
-      </c>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="42"/>
       <c r="K43" s="21"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="23">
-        <f>SUM(G43:G43)</f>
+        <v>65</v>
+      </c>
+      <c r="C44" s="19">
+        <v>1</v>
+      </c>
+      <c r="D44" s="39">
         <v>3</v>
       </c>
-      <c r="H44" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I44" s="23">
-        <v>6152.23</v>
-      </c>
-      <c r="J44" s="42">
-        <f>G44*I44</f>
-        <v>18456.689999999999</v>
-      </c>
+      <c r="E44" s="39">
+        <v>1</v>
+      </c>
+      <c r="F44" s="39">
+        <v>1</v>
+      </c>
+      <c r="G44" s="40">
+        <f t="shared" ref="G44" si="0">PRODUCT(C44:F44)</f>
+        <v>3</v>
+      </c>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
       <c r="K44" s="21"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="20"/>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="23"/>
+      <c r="G45" s="23">
+        <f>SUM(G44:G44)</f>
+        <v>3</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I45" s="23">
+        <v>6152.23</v>
+      </c>
       <c r="J45" s="42">
-        <f>0.13*G44*26798.3/6</f>
-        <v>1741.8895</v>
+        <f>G45*I45</f>
+        <v>18456.689999999999</v>
       </c>
       <c r="K45" s="21"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
-      <c r="B46" s="38"/>
+      <c r="B46" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C46" s="19"/>
       <c r="D46" s="20"/>
       <c r="E46" s="21"/>
@@ -2806,14 +2828,15 @@
       <c r="G46" s="23"/>
       <c r="H46" s="22"/>
       <c r="I46" s="23"/>
-      <c r="J46" s="42"/>
+      <c r="J46" s="42">
+        <f>0.13*G45*26798.3/6</f>
+        <v>1741.8895</v>
+      </c>
       <c r="K46" s="21"/>
     </row>
-    <row r="47" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
-      <c r="B47" s="30" t="s">
-        <v>68</v>
-      </c>
+      <c r="B47" s="38"/>
       <c r="C47" s="19"/>
       <c r="D47" s="20"/>
       <c r="E47" s="21"/>
@@ -2824,33 +2847,28 @@
       <c r="J47" s="42"/>
       <c r="K47" s="21"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="18"/>
-      <c r="B48" s="38" t="s">
+    <row r="48" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
+        <v>8</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="23"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="21"/>
+    </row>
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="19">
-        <v>1</v>
-      </c>
-      <c r="D48" s="39">
-        <v>3</v>
-      </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39">
-        <v>2</v>
-      </c>
-      <c r="G48" s="40">
-        <f t="shared" ref="G48:G49" si="1">PRODUCT(C48:F48)</f>
-        <v>6</v>
-      </c>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="21"/>
-    </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18"/>
-      <c r="B49" s="38"/>
       <c r="C49" s="19">
         <v>1</v>
       </c>
@@ -2859,63 +2877,69 @@
       </c>
       <c r="E49" s="39"/>
       <c r="F49" s="39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" s="40">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f t="shared" ref="G49:G50" si="1">PRODUCT(C49:F49)</f>
+        <v>6</v>
       </c>
       <c r="H49" s="41"/>
       <c r="I49" s="41"/>
       <c r="J49" s="41"/>
       <c r="K49" s="21"/>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
-      <c r="B50" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="23">
-        <f>SUM(G48:G49)</f>
-        <v>9</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I50" s="23">
-        <v>161.41999999999999</v>
-      </c>
-      <c r="J50" s="42">
-        <f>G50*I50</f>
-        <v>1452.78</v>
-      </c>
+      <c r="B50" s="38"/>
+      <c r="C50" s="19">
+        <v>1</v>
+      </c>
+      <c r="D50" s="39">
+        <v>3</v>
+      </c>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39">
+        <v>1</v>
+      </c>
+      <c r="G50" s="40">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="41"/>
       <c r="K50" s="21"/>
     </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="20"/>
       <c r="E51" s="21"/>
       <c r="F51" s="21"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="23"/>
+      <c r="G51" s="23">
+        <f>SUM(G49:G50)</f>
+        <v>9</v>
+      </c>
+      <c r="H51" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I51" s="23">
+        <v>161.41999999999999</v>
+      </c>
       <c r="J51" s="42">
-        <f>0.13*G50*45360/300</f>
-        <v>176.904</v>
+        <f>G51*I51</f>
+        <v>1452.78</v>
       </c>
       <c r="K51" s="21"/>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
-      <c r="B52" s="38"/>
+      <c r="B52" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="C52" s="19"/>
       <c r="D52" s="20"/>
       <c r="E52" s="21"/>
@@ -2923,150 +2947,145 @@
       <c r="G52" s="23"/>
       <c r="H52" s="22"/>
       <c r="I52" s="23"/>
-      <c r="J52" s="42"/>
+      <c r="J52" s="42">
+        <f>0.13*G51*45360/300</f>
+        <v>176.904</v>
+      </c>
       <c r="K52" s="21"/>
     </row>
-    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="18">
-        <v>12</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C53" s="19">
-        <v>1</v>
-      </c>
+    <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="19"/>
       <c r="D53" s="20"/>
       <c r="E53" s="21"/>
       <c r="F53" s="21"/>
-      <c r="G53" s="35">
-        <f t="shared" ref="G53" si="2">PRODUCT(C53:F53)</f>
+      <c r="G53" s="23"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="42"/>
+      <c r="K53" s="21"/>
+    </row>
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="18">
+        <v>9</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="19">
         <v>1</v>
       </c>
-      <c r="H53" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I53" s="23">
-        <v>500</v>
-      </c>
-      <c r="J53" s="35">
-        <f>G53*I53</f>
-        <v>500</v>
-      </c>
-      <c r="K53" s="21"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="25"/>
-      <c r="S53" s="25"/>
-    </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="19"/>
       <c r="D54" s="20"/>
       <c r="E54" s="21"/>
       <c r="F54" s="21"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="42"/>
+      <c r="G54" s="35">
+        <f t="shared" ref="G54" si="2">PRODUCT(C54:F54)</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="23">
+        <v>500</v>
+      </c>
+      <c r="J54" s="35">
+        <f>G54*I54</f>
+        <v>500</v>
+      </c>
       <c r="K54" s="21"/>
       <c r="M54" s="25"/>
-      <c r="N54" s="1">
-        <f>2.4*3.281</f>
-        <v>7.8743999999999996</v>
-      </c>
+      <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="25"/>
       <c r="S54" s="25"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="41"/>
-      <c r="B55" s="47" t="s">
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="42"/>
+      <c r="K55" s="21"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="1">
+        <f>2.4*3.281</f>
+        <v>7.8743999999999996</v>
+      </c>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="25"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="41"/>
+      <c r="B56" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="48"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="42"/>
-      <c r="J55" s="42">
-        <f>SUM(J10:J53)</f>
-        <v>240120.72386825923</v>
-      </c>
-      <c r="K55" s="37"/>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="59"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="63"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="60"/>
-      <c r="F56" s="60"/>
-      <c r="G56" s="61"/>
-      <c r="H56" s="61"/>
-      <c r="I56" s="61"/>
-      <c r="J56" s="61"/>
-      <c r="K56" s="58"/>
-    </row>
-    <row r="57" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="51"/>
-      <c r="B57" s="29" t="s">
+      <c r="C56" s="48"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="42"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="42"/>
+      <c r="J56" s="42">
+        <f>SUM(J10:J54)</f>
+        <v>226825.43584109875</v>
+      </c>
+      <c r="K56" s="37"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="59"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="63"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="61"/>
+      <c r="I57" s="61"/>
+      <c r="J57" s="61"/>
+      <c r="K57" s="58"/>
+    </row>
+    <row r="58" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="51"/>
+      <c r="B58" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="83">
-        <f>J55</f>
-        <v>240120.72386825923</v>
-      </c>
-      <c r="D57" s="83"/>
-      <c r="E57" s="40">
+      <c r="C58" s="88">
+        <f>J56</f>
+        <v>226825.43584109875</v>
+      </c>
+      <c r="D58" s="88"/>
+      <c r="E58" s="40">
         <v>100</v>
       </c>
-      <c r="F57" s="52"/>
-      <c r="G57" s="53"/>
-      <c r="H57" s="52"/>
-      <c r="I57" s="54"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="56"/>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="57"/>
-      <c r="B58" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="86">
-        <v>200000</v>
-      </c>
-      <c r="D58" s="86"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="50"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="50"/>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F58" s="52"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="54"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="56"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="57"/>
       <c r="B59" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="86">
-        <f>C58-C61-C62</f>
-        <v>190000</v>
-      </c>
-      <c r="D59" s="86"/>
-      <c r="E59" s="40">
-        <f>C59/C57*100</f>
-        <v>79.126864578436951</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C59" s="91">
+        <v>200000</v>
+      </c>
+      <c r="D59" s="91"/>
+      <c r="E59" s="40"/>
       <c r="F59" s="50"/>
       <c r="G59" s="49"/>
       <c r="H59" s="49"/>
@@ -3074,19 +3093,19 @@
       <c r="J59" s="49"/>
       <c r="K59" s="50"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="57"/>
       <c r="B60" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="83">
-        <f>C57-C59</f>
-        <v>50120.723868259229</v>
-      </c>
-      <c r="D60" s="83"/>
+        <v>33</v>
+      </c>
+      <c r="C60" s="91">
+        <f>C59-C62-C63</f>
+        <v>190000</v>
+      </c>
+      <c r="D60" s="91"/>
       <c r="E60" s="40">
-        <f>100-E59</f>
-        <v>20.873135421563049</v>
+        <f>C60/C58*100</f>
+        <v>83.764856130642869</v>
       </c>
       <c r="F60" s="50"/>
       <c r="G60" s="49"/>
@@ -3095,18 +3114,19 @@
       <c r="J60" s="49"/>
       <c r="K60" s="50"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="57"/>
       <c r="B61" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="83">
-        <f>C58*0.03</f>
-        <v>6000</v>
-      </c>
-      <c r="D61" s="83"/>
+        <v>34</v>
+      </c>
+      <c r="C61" s="88">
+        <f>C58-C60</f>
+        <v>36825.435841098748</v>
+      </c>
+      <c r="D61" s="88"/>
       <c r="E61" s="40">
-        <v>3</v>
+        <f>100-E60</f>
+        <v>16.235143869357131</v>
       </c>
       <c r="F61" s="50"/>
       <c r="G61" s="49"/>
@@ -3115,18 +3135,18 @@
       <c r="J61" s="49"/>
       <c r="K61" s="50"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="57"/>
       <c r="B62" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="83">
-        <f>C58*0.02</f>
-        <v>4000</v>
-      </c>
-      <c r="D62" s="83"/>
+        <v>35</v>
+      </c>
+      <c r="C62" s="88">
+        <f>C59*0.03</f>
+        <v>6000</v>
+      </c>
+      <c r="D62" s="88"/>
       <c r="E62" s="40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F62" s="50"/>
       <c r="G62" s="49"/>
@@ -3135,78 +3155,106 @@
       <c r="J62" s="49"/>
       <c r="K62" s="50"/>
     </row>
-    <row r="63" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="58"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
-      <c r="F63" s="58"/>
-      <c r="G63" s="58"/>
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
-      <c r="J63" s="58"/>
-      <c r="K63" s="58"/>
-    </row>
-    <row r="64" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A63" s="57"/>
+      <c r="B63" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="88">
+        <f>C59*0.02</f>
+        <v>4000</v>
+      </c>
+      <c r="D63" s="88"/>
+      <c r="E63" s="40">
+        <v>2</v>
+      </c>
+      <c r="F63" s="50"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="50"/>
+    </row>
+    <row r="64" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="58"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="58"/>
+      <c r="F64" s="58"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="58"/>
+      <c r="J64" s="58"/>
+      <c r="K64" s="58"/>
+    </row>
+    <row r="65" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="O14:U14"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="O15:U15"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -3214,14 +3262,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>